<commit_message>
final change before release
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sup\Documents\UiPath\Generate Yearly Report\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4439915F-E4B3-4207-B7CE-CC6A5FD1743C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D2C6913-1618-41C7-90F0-6ED590F40836}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -130,9 +130,6 @@
     <t>Year</t>
   </si>
   <si>
-    <t>/Data/Temp/Reports</t>
-  </si>
-  <si>
     <t>Temp report path</t>
   </si>
   <si>
@@ -140,6 +137,9 @@
   </si>
   <si>
     <t>ACME Web Application URL</t>
+  </si>
+  <si>
+    <t>\Data\Temp\Rawreports\</t>
   </si>
 </sst>
 </file>
@@ -529,7 +529,7 @@
   <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -593,7 +593,7 @@
         <v>29</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -612,10 +612,10 @@
         <v>32</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
@@ -626,7 +626,7 @@
         <v>2019</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Simulate Click disabled for Upload work item
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sup\Documents\UiPath\Generate Yearly Report\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D2C6913-1618-41C7-90F0-6ED590F40836}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4DB8567-5FC0-49FB-8074-7C334D84BA28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -115,31 +115,31 @@
     <t>https://acme-test.uipath.com</t>
   </si>
   <si>
+    <t>Orchestrator Asset Name</t>
+  </si>
+  <si>
+    <t>Raw_ReportPath</t>
+  </si>
+  <si>
+    <t>GenerateYearlyReportforVendor</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Temp report path</t>
+  </si>
+  <si>
+    <t>Year of report</t>
+  </si>
+  <si>
+    <t>ACME Web Application URL</t>
+  </si>
+  <si>
+    <t>\Data\Temp\Rawreports\</t>
+  </si>
+  <si>
     <t>acme_system</t>
-  </si>
-  <si>
-    <t>Orchestrator Asset Name</t>
-  </si>
-  <si>
-    <t>Raw_ReportPath</t>
-  </si>
-  <si>
-    <t>GenerateYearlyReportforVendor</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Temp report path</t>
-  </si>
-  <si>
-    <t>Year of report</t>
-  </si>
-  <si>
-    <t>ACME Web Application URL</t>
-  </si>
-  <si>
-    <t>\Data\Temp\Rawreports\</t>
   </si>
 </sst>
 </file>
@@ -529,7 +529,7 @@
   <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -579,7 +579,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>21</v>
@@ -593,7 +593,7 @@
         <v>29</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -601,32 +601,32 @@
         <v>28</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="6">
         <v>2019</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>